<commit_message>
added modified excel file
</commit_message>
<xml_diff>
--- a/ExcelFiles/OrangeHRMTestData.xlsx
+++ b/ExcelFiles/OrangeHRMTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OrangeHRMTask\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3F8CBA-BC12-412D-893B-1E3A5DE5AA11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4611AB-B3AF-4322-BED4-7C9FF96A0925}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{437D755A-BBE0-4A18-A3EC-E56A64BAA2FD}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>Id</t>
   </si>
   <si>
-    <t>0247</t>
-  </si>
-  <si>
     <t>rajad675</t>
+  </si>
+  <si>
+    <t>0263</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,7 +575,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>17</v>
@@ -584,7 +584,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>